<commit_message>
Finished Main Admin Filtering
</commit_message>
<xml_diff>
--- a/public/storage/main-admin-report.xlsx
+++ b/public/storage/main-admin-report.xlsx
@@ -4,6 +4,10 @@
   <sheets>
     <sheet name="Tickets" sheetId="1" r:id="rIdSheet1" state="visible"/>
     <sheet name="Staff Status" sheetId="2" r:id="rIdSheet2" state="visible"/>
+    <sheet name="Queue Counts" sheetId="3" r:id="rIdSheet3" state="visible"/>
+    <sheet name="Staff Leaderboards" sheetId="4" r:id="rIdSheet4" state="visible"/>
+    <sheet name="Occupied Departments" sheetId="5" r:id="rIdSheet5" state="visible"/>
+    <sheet name="Feedbacks" sheetId="6" r:id="rIdSheet6" state="visible"/>
   </sheets>
 </workbook>
 </file>
@@ -18,6 +22,42 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Unknown</author>
+  </authors>
+  <commentList>    </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Unknown</author>
+  </authors>
+  <commentList>    </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Unknown</author>
+  </authors>
+  <commentList>    </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Unknown</author>
+  </authors>
+  <commentList>    </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Unknown</author>
@@ -116,27 +156,27 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Jane Doe</t>
+          <t>John Doe</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>Senior High School</t>
+          <t>Graduate School</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>Accountancy, Business, and Management Strand</t>
+          <t>Master</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>Complete</t>
+          <t>Pending</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>2023-04-26 21:49:26</t>
+          <t>2023-04-21 14:07:35</t>
         </is>
       </c>
       <c r="G2" s="0">
@@ -146,36 +186,176 @@
     <row r="3" spans="1:7" customHeight="0">
       <c r="A3" s="0" t="inlineStr">
         <is>
+          <t>R002</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Jane Doe</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>Bachelor of Science in Information Technology</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>2023-04-21 14:16:39</t>
+        </is>
+      </c>
+      <c r="G3" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" customHeight="0">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>R003</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Frank Doe</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>Senior High School</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>Accountancy, Business, and Management Strand</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>2023-04-21 14:18:33</t>
+        </is>
+      </c>
+      <c r="G4" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" customHeight="0">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>R004</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Hank Doe</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>Junior High School</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>Junior High School</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>2023-04-21 14:19:30</t>
+        </is>
+      </c>
+      <c r="G5" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" customHeight="0">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>R005</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Sam Doe</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>Graduate School</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>2023-04-21 14:41:02</t>
+        </is>
+      </c>
+      <c r="G6" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" customHeight="0">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
           <t>R001</t>
         </is>
       </c>
-      <c r="B3" s="0" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-      <c r="C3" s="0" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>Frank Doe</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
         <is>
           <t>College</t>
         </is>
       </c>
-      <c r="D3" s="0" t="inlineStr">
+      <c r="D7" s="0" t="inlineStr">
         <is>
           <t>Bachelor of Science in Information Technology</t>
         </is>
       </c>
-      <c r="E3" s="0" t="inlineStr">
-        <is>
-          <t>Complete</t>
-        </is>
-      </c>
-      <c r="F3" s="0" t="inlineStr">
-        <is>
-          <t>2023-04-27 11:00:59</t>
-        </is>
-      </c>
-      <c r="G3" s="0">
-        <v>6</v>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>Pending</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>2023-05-27 11:00:59</t>
+        </is>
+      </c>
+      <c r="G7" s="0">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -206,12 +386,12 @@
     <row r="2" spans="1:3" customHeight="0">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>Mr. Mortimer Parker</t>
+          <t>Roma VonRueden</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>Cashier</t>
+          <t>Registrar</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
@@ -223,17 +403,239 @@
     <row r="3" spans="1:3" customHeight="0">
       <c r="A3" s="0" t="inlineStr">
         <is>
+          <t>Reese Harris</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Registrar</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>Logged Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" spans="1:3" customHeight="0">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>Mr. Mortimer Parker</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Cashier</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>Logged Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" spans="1:3" customHeight="0">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
           <t>Jermey Tremblay II</t>
         </is>
       </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Cashier</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>Logged Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" spans="1:3" customHeight="0">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>Prof. Lexi Mayert</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>College Library</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>Logged Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" spans="1:3" customHeight="0">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>Rosa Auer</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>High School Library</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>Logged Out</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <legacyDrawing r:id="rId_comments_vml1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetData>
+    <row r="1" spans="1:1" customHeight="0">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Total Queues</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:1" customHeight="0">
+      <c r="A2" s="0">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <legacyDrawing r:id="rId_comments_vml1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetData>
+    <row r="1" spans="1:3" customHeight="0">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>Total Served</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customHeight="0">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>Reese Harris</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Registrar</t>
+        </is>
+      </c>
+      <c r="C2" s="0">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" customHeight="0">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>Jermey Tremblay II</t>
+        </is>
+      </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
           <t>Cashier</t>
         </is>
       </c>
+      <c r="C3" s="0">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <legacyDrawing r:id="rId_comments_vml1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetData>
+    <row r="1" spans="1:1" customHeight="0">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Total Occupied Departments</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:1" customHeight="0">
+      <c r="A2" s="0">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <legacyDrawing r:id="rId_comments_vml1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetData>
+    <row r="1" spans="1:3" customHeight="0">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>Feedback</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>Date Sent</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:3" customHeight="0">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <t>Anonymous</t>
+        </is>
+      </c>
+      <c r="B2" s="0" t="inlineStr">
+        <is>
+          <t>Hakdog</t>
+        </is>
+      </c>
+      <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>2023-04-28 15:10:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" spans="1:3" customHeight="0">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>Anonymous</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>ay weh?</t>
+        </is>
+      </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>Logged Out</t>
+          <t>2023-04-28 15:11:11</t>
         </is>
       </c>
     </row>

</xml_diff>